<commit_message>
Updated CMs with Family feature for combined models
</commit_message>
<xml_diff>
--- a/SegmentedConfusionMatrices.xlsx
+++ b/SegmentedConfusionMatrices.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ethan\Documents\Ethan\TMG\Research\PORPOS-TMG\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D8AC4C1-DC72-4F62-A0C9-DF54CAD9890F}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8D8223E-1AC9-4F94-A2F0-10D4F440D834}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" xr2:uid="{A25D8D46-635A-47F6-90AA-F320D2055949}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" firstSheet="3" activeTab="7" xr2:uid="{A25D8D46-635A-47F6-90AA-F320D2055949}"/>
   </bookViews>
   <sheets>
     <sheet name="Logit-Hardmax" sheetId="1" r:id="rId1"/>
@@ -539,7 +539,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61E5D915-47C2-4B68-88FC-9CA9AAB36509}">
   <dimension ref="A2:N44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
@@ -3327,8 +3327,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04AD215D-9733-4714-933F-30B2D615CA7E}">
   <dimension ref="A2:N44"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4:B10"/>
+    <sheetView topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="C34" sqref="C34:C40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4301,7 +4301,7 @@
         <v>4</v>
       </c>
       <c r="C34" s="13">
-        <v>150</v>
+        <v>131</v>
       </c>
       <c r="D34" s="10">
         <v>0</v>
@@ -4310,28 +4310,28 @@
         <v>12</v>
       </c>
       <c r="F34" s="10">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G34" s="10">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="H34" s="10">
         <v>0</v>
       </c>
       <c r="I34" s="10">
-        <v>45</v>
+        <v>51</v>
       </c>
       <c r="J34" s="12">
         <f>SUM(C34:I34)</f>
-        <v>282</v>
+        <v>263</v>
       </c>
       <c r="K34" s="9">
         <f>C34/J34</f>
-        <v>0.53191489361702127</v>
+        <v>0.49809885931558934</v>
       </c>
       <c r="M34" s="3">
         <f>AVERAGE(K34:K40)</f>
-        <v>0.31337060846577858</v>
+        <v>0.3225455164931908</v>
       </c>
       <c r="N34" s="2" t="s">
         <v>12</v>
@@ -4348,23 +4348,23 @@
         <v>0</v>
       </c>
       <c r="E35" s="10">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="F35" s="10">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G35" s="10">
-        <v>86</v>
+        <v>96</v>
       </c>
       <c r="H35" s="10">
         <v>0</v>
       </c>
       <c r="I35" s="10">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="J35" s="12">
         <f t="shared" ref="J35:J40" si="6">SUM(C35:I35)</f>
-        <v>127</v>
+        <v>152</v>
       </c>
       <c r="K35" s="9">
         <f>D35/J35</f>
@@ -4372,7 +4372,7 @@
       </c>
       <c r="M35" s="3">
         <f>AVERAGE(C42:I42)</f>
-        <v>0.42524732686265959</v>
+        <v>0.44554720542583975</v>
       </c>
       <c r="N35" s="2" t="s">
         <v>14</v>
@@ -4383,37 +4383,37 @@
         <v>6</v>
       </c>
       <c r="C36" s="10">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="D36" s="10">
         <v>0</v>
       </c>
       <c r="E36" s="13">
-        <v>61</v>
+        <v>103</v>
       </c>
       <c r="F36" s="10">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="G36" s="10">
-        <v>445</v>
+        <v>415</v>
       </c>
       <c r="H36" s="10">
         <v>0</v>
       </c>
       <c r="I36" s="10">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="J36" s="12">
         <f t="shared" si="6"/>
-        <v>821</v>
+        <v>828</v>
       </c>
       <c r="K36" s="9">
         <f>E36/J36</f>
-        <v>7.4299634591961025E-2</v>
+        <v>0.12439613526570048</v>
       </c>
       <c r="M36" s="4">
         <f>2*M34*M35/(M34+M35)</f>
-        <v>0.36083611619352651</v>
+        <v>0.37419767013838356</v>
       </c>
       <c r="N36" s="2" t="s">
         <v>15</v>
@@ -4424,37 +4424,37 @@
         <v>7</v>
       </c>
       <c r="C37" s="10">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D37" s="10">
         <v>0</v>
       </c>
       <c r="E37" s="10">
-        <v>10</v>
+        <v>41</v>
       </c>
       <c r="F37" s="13">
-        <v>93</v>
+        <v>120</v>
       </c>
       <c r="G37" s="10">
-        <v>147</v>
+        <v>124</v>
       </c>
       <c r="H37" s="10">
         <v>0</v>
       </c>
       <c r="I37" s="10">
-        <v>62</v>
+        <v>45</v>
       </c>
       <c r="J37" s="12">
         <f t="shared" si="6"/>
-        <v>317</v>
+        <v>332</v>
       </c>
       <c r="K37" s="9">
         <f>F37/J37</f>
-        <v>0.29337539432176657</v>
+        <v>0.36144578313253012</v>
       </c>
       <c r="M37" s="4">
         <f>SUM(C34,D35,E36,F37,G38,H39,I40)/J41</f>
-        <v>0.48480662983425415</v>
+        <v>0.48342541436464087</v>
       </c>
       <c r="N37" s="2" t="s">
         <v>13</v>
@@ -4465,36 +4465,36 @@
         <v>8</v>
       </c>
       <c r="C38" s="10">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="D38" s="10">
         <v>0</v>
       </c>
       <c r="E38" s="10">
-        <v>53</v>
+        <v>106</v>
       </c>
       <c r="F38" s="10">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="G38" s="13">
-        <v>1370</v>
+        <v>1315</v>
       </c>
       <c r="H38" s="10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I38" s="10">
-        <v>213</v>
+        <v>198</v>
       </c>
       <c r="J38" s="12">
         <f t="shared" si="6"/>
-        <v>1765</v>
+        <v>1742</v>
       </c>
       <c r="K38" s="9">
         <f>G38/J38</f>
-        <v>0.77620396600566577</v>
+        <v>0.7548794489092997</v>
       </c>
       <c r="M38" s="4">
-        <v>0.37902058698336599</v>
+        <v>0.37382768003030098</v>
       </c>
       <c r="N38" s="2" t="s">
         <v>16</v>
@@ -4505,33 +4505,33 @@
         <v>9</v>
       </c>
       <c r="C39" s="10">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D39" s="10">
         <v>0</v>
       </c>
       <c r="E39" s="10">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F39" s="10">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="G39" s="10">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="H39" s="13">
         <v>6</v>
       </c>
       <c r="I39" s="10">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="J39" s="12">
         <f t="shared" si="6"/>
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="K39" s="9">
         <f>H39/J39</f>
-        <v>6.3157894736842107E-2</v>
+        <v>6.25E-2</v>
       </c>
     </row>
     <row r="40" spans="2:14" x14ac:dyDescent="0.35">
@@ -4539,33 +4539,33 @@
         <v>10</v>
       </c>
       <c r="C40" s="10">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="D40" s="10">
         <v>0</v>
       </c>
       <c r="E40" s="10">
-        <v>23</v>
+        <v>50</v>
       </c>
       <c r="F40" s="10">
-        <v>24</v>
+        <v>39</v>
       </c>
       <c r="G40" s="10">
-        <v>376</v>
+        <v>334</v>
       </c>
       <c r="H40" s="10">
         <v>0</v>
       </c>
       <c r="I40" s="13">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="J40" s="12">
         <f t="shared" si="6"/>
-        <v>937</v>
+        <v>931</v>
       </c>
       <c r="K40" s="9">
         <f>I40/J40</f>
-        <v>0.45464247598719315</v>
+        <v>0.4564983888292159</v>
       </c>
     </row>
     <row r="41" spans="2:14" x14ac:dyDescent="0.35">
@@ -4574,7 +4574,7 @@
       </c>
       <c r="C41" s="12">
         <f>SUM(C34:C40)</f>
-        <v>434</v>
+        <v>407</v>
       </c>
       <c r="D41" s="12">
         <f t="shared" ref="D41:I41" si="7">SUM(D34:D40)</f>
@@ -4582,23 +4582,23 @@
       </c>
       <c r="E41" s="12">
         <f t="shared" si="7"/>
-        <v>172</v>
+        <v>337</v>
       </c>
       <c r="F41" s="12">
         <f t="shared" si="7"/>
-        <v>209</v>
+        <v>241</v>
       </c>
       <c r="G41" s="12">
         <f t="shared" si="7"/>
-        <v>2545</v>
+        <v>2398</v>
       </c>
       <c r="H41" s="12">
         <f t="shared" si="7"/>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="I41" s="12">
         <f t="shared" si="7"/>
-        <v>977</v>
+        <v>955</v>
       </c>
       <c r="J41" s="12">
         <f>SUM(J34:J40)</f>
@@ -4612,7 +4612,7 @@
       </c>
       <c r="C42" s="9">
         <f>C34/C41</f>
-        <v>0.34562211981566821</v>
+        <v>0.32186732186732187</v>
       </c>
       <c r="D42" s="9">
         <f>IFERROR(D35/D41, 0)</f>
@@ -4620,23 +4620,23 @@
       </c>
       <c r="E42" s="9">
         <f>IFERROR(E36/E41, 0)</f>
-        <v>0.35465116279069769</v>
+        <v>0.3056379821958457</v>
       </c>
       <c r="F42" s="9">
         <f>IFERROR(F37/F41, 0)</f>
-        <v>0.44497607655502391</v>
+        <v>0.49792531120331951</v>
       </c>
       <c r="G42" s="9">
         <f>IFERROR(G38/G41, 0)</f>
-        <v>0.53831041257367385</v>
+        <v>0.54837364470391992</v>
       </c>
       <c r="H42" s="9">
         <f>IFERROR(H39/H41, 0)</f>
-        <v>0.8571428571428571</v>
+        <v>1</v>
       </c>
       <c r="I42" s="9">
         <f>IFERROR(I40/I41, 0)</f>
-        <v>0.436028659160696</v>
+        <v>0.44502617801047123</v>
       </c>
       <c r="J42" s="10"/>
       <c r="K42" s="10"/>
@@ -4647,31 +4647,31 @@
       </c>
       <c r="C43" s="10">
         <f>C41-J34</f>
-        <v>152</v>
+        <v>144</v>
       </c>
       <c r="D43" s="10">
         <f>D41-J35</f>
-        <v>-127</v>
+        <v>-152</v>
       </c>
       <c r="E43" s="10">
         <f>E41-J36</f>
-        <v>-649</v>
+        <v>-491</v>
       </c>
       <c r="F43" s="10">
         <f>F41-J37</f>
-        <v>-108</v>
+        <v>-91</v>
       </c>
       <c r="G43" s="10">
         <f>G41-J38</f>
-        <v>780</v>
+        <v>656</v>
       </c>
       <c r="H43" s="10">
         <f>H41-J39</f>
-        <v>-88</v>
+        <v>-90</v>
       </c>
       <c r="I43" s="10">
         <f>I41-J40</f>
-        <v>40</v>
+        <v>24</v>
       </c>
       <c r="J43" s="10"/>
       <c r="K43" s="10"/>
@@ -4682,31 +4682,31 @@
       </c>
       <c r="C44" s="9">
         <f>C43/$J41</f>
-        <v>3.4990791896869246E-2</v>
+        <v>3.3149171270718231E-2</v>
       </c>
       <c r="D44" s="9">
         <f t="shared" ref="D44:I44" si="8">D43/$J41</f>
-        <v>-2.9235727440147331E-2</v>
+        <v>-3.4990791896869246E-2</v>
       </c>
       <c r="E44" s="9">
         <f t="shared" si="8"/>
-        <v>-0.14940147329650091</v>
+        <v>-0.11302946593001842</v>
       </c>
       <c r="F44" s="9">
         <f t="shared" si="8"/>
-        <v>-2.4861878453038673E-2</v>
+        <v>-2.094843462246777E-2</v>
       </c>
       <c r="G44" s="9">
         <f t="shared" si="8"/>
-        <v>0.17955801104972377</v>
+        <v>0.15101289134438306</v>
       </c>
       <c r="H44" s="9">
         <f t="shared" si="8"/>
-        <v>-2.0257826887661142E-2</v>
+        <v>-2.0718232044198894E-2</v>
       </c>
       <c r="I44" s="9">
         <f t="shared" si="8"/>
-        <v>9.2081031307550652E-3</v>
+        <v>5.5248618784530384E-3</v>
       </c>
       <c r="J44" s="10"/>
       <c r="K44" s="10"/>
@@ -4721,8 +4721,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B505794A-6DC4-4723-AC7C-CF972A3E9EAC}">
   <dimension ref="A2:N44"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B34" sqref="B34:B40"/>
+    <sheetView topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="C34" sqref="C34:C40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5695,37 +5695,37 @@
         <v>4</v>
       </c>
       <c r="C34" s="6">
-        <v>79.169448465864903</v>
+        <v>75.966938713914899</v>
       </c>
       <c r="D34" s="7">
-        <v>7.0702606607917602</v>
+        <v>6.0312824046856299</v>
       </c>
       <c r="E34" s="7">
-        <v>53.79215965865</v>
+        <v>48.614268857627899</v>
       </c>
       <c r="F34" s="7">
-        <v>5.4661037055049198</v>
+        <v>4.7071085878025603</v>
       </c>
       <c r="G34" s="7">
-        <v>73.997590499124797</v>
+        <v>68.801462231566504</v>
       </c>
       <c r="H34" s="7">
-        <v>4.9339148020385499</v>
+        <v>4.6168864402638103</v>
       </c>
       <c r="I34" s="7">
-        <v>57.570522208024897</v>
+        <v>54.262052764138602</v>
       </c>
       <c r="J34" s="12">
         <f>SUM(C34:I34)</f>
-        <v>281.99999999999983</v>
+        <v>262.99999999999989</v>
       </c>
       <c r="K34" s="9">
         <f>C34/J34</f>
-        <v>0.28074272505625869</v>
+        <v>0.28884767571830772</v>
       </c>
       <c r="M34" s="3">
         <f>AVERAGE(K34:K40)</f>
-        <v>0.25409266782184425</v>
+        <v>0.25829989181690693</v>
       </c>
       <c r="N34" s="2" t="s">
         <v>12</v>
@@ -5736,37 +5736,37 @@
         <v>5</v>
       </c>
       <c r="C35" s="7">
-        <v>6.6576922651996</v>
+        <v>8.0893458975113894</v>
       </c>
       <c r="D35" s="6">
-        <v>5.7392101034285998</v>
+        <v>6.3145314835273298</v>
       </c>
       <c r="E35" s="7">
-        <v>26.234005583563999</v>
+        <v>32.474140950572199</v>
       </c>
       <c r="F35" s="7">
-        <v>7.6245356745886204</v>
+        <v>10.0495423234445</v>
       </c>
       <c r="G35" s="7">
-        <v>56.4113229752409</v>
+        <v>64.995049698884401</v>
       </c>
       <c r="H35" s="7">
-        <v>2.34693554287455</v>
+        <v>2.85387986556275</v>
       </c>
       <c r="I35" s="7">
-        <v>21.9862978551037</v>
+        <v>27.2235097804971</v>
       </c>
       <c r="J35" s="12">
         <f t="shared" ref="J35:J40" si="6">SUM(C35:I35)</f>
-        <v>126.99999999999997</v>
+        <v>151.99999999999966</v>
       </c>
       <c r="K35" s="9">
         <f>D35/J35</f>
-        <v>4.519063073565828E-2</v>
+        <v>4.1542970286364105E-2</v>
       </c>
       <c r="M35" s="3">
         <f>AVERAGE(C42:I42)</f>
-        <v>0.2551508975914018</v>
+        <v>0.25563622656878321</v>
       </c>
       <c r="N35" s="2" t="s">
         <v>14</v>
@@ -5777,37 +5777,37 @@
         <v>6</v>
       </c>
       <c r="C36" s="7">
-        <v>52.110037522976498</v>
+        <v>57.606613660246801</v>
       </c>
       <c r="D36" s="7">
-        <v>30.450985473893901</v>
+        <v>27.359677668758</v>
       </c>
       <c r="E36" s="6">
-        <v>182.47810744041601</v>
+        <v>188.97166672243</v>
       </c>
       <c r="F36" s="7">
-        <v>64.178401264414106</v>
+        <v>61.415607864844503</v>
       </c>
       <c r="G36" s="7">
-        <v>304.76157782162801</v>
+        <v>301.25746340272201</v>
       </c>
       <c r="H36" s="7">
-        <v>17.813745770642299</v>
+        <v>18.778281413989699</v>
       </c>
       <c r="I36" s="7">
-        <v>169.207144706028</v>
+        <v>172.61068926700699</v>
       </c>
       <c r="J36" s="12">
         <f t="shared" si="6"/>
-        <v>820.99999999999886</v>
+        <v>827.99999999999795</v>
       </c>
       <c r="K36" s="9">
         <f>E36/J36</f>
-        <v>0.2222632246533694</v>
+        <v>0.22822665063095468</v>
       </c>
       <c r="M36" s="4">
         <f>2*M34*M35/(M34+M35)</f>
-        <v>0.25462068318340736</v>
+        <v>0.25696115647449136</v>
       </c>
       <c r="N36" s="2" t="s">
         <v>15</v>
@@ -5818,37 +5818,37 @@
         <v>7</v>
       </c>
       <c r="C37" s="7">
-        <v>6.5660540966091103</v>
+        <v>6.2455382420977097</v>
       </c>
       <c r="D37" s="7">
-        <v>8.8183009205950604</v>
+        <v>8.27366887227093</v>
       </c>
       <c r="E37" s="7">
-        <v>58.385155251152298</v>
+        <v>65.166312584660204</v>
       </c>
       <c r="F37" s="6">
-        <v>84.342427032549395</v>
+        <v>97.441371177474906</v>
       </c>
       <c r="G37" s="7">
-        <v>90.091733002294504</v>
+        <v>87.439029988439898</v>
       </c>
       <c r="H37" s="7">
-        <v>7.7529439846712496</v>
+        <v>7.9243425566794103</v>
       </c>
       <c r="I37" s="7">
-        <v>61.043385712128099</v>
+        <v>59.509736578376803</v>
       </c>
       <c r="J37" s="12">
         <f t="shared" si="6"/>
-        <v>316.99999999999977</v>
+        <v>331.99999999999989</v>
       </c>
       <c r="K37" s="9">
         <f>F37/J37</f>
-        <v>0.26606443858848411</v>
+        <v>0.29349810595624981</v>
       </c>
       <c r="M37" s="4">
         <f>SUM(C34,D35,E36,F37,G38,H39,I40)/J41</f>
-        <v>0.37902058698336877</v>
+        <v>0.37382768003030092</v>
       </c>
       <c r="N37" s="2" t="s">
         <v>13</v>
@@ -5859,36 +5859,36 @@
         <v>8</v>
       </c>
       <c r="C38" s="7">
-        <v>68.225312076070793</v>
+        <v>75.212843622185503</v>
       </c>
       <c r="D38" s="7">
-        <v>58.845047888918899</v>
+        <v>57.721651411866503</v>
       </c>
       <c r="E38" s="7">
-        <v>288.30188117721201</v>
+        <v>291.65504397300401</v>
       </c>
       <c r="F38" s="7">
-        <v>85.5954771486483</v>
+        <v>89.225660335154302</v>
       </c>
       <c r="G38" s="6">
-        <v>967.25528228551195</v>
+        <v>927.34009549255597</v>
       </c>
       <c r="H38" s="7">
-        <v>28.7407834315614</v>
+        <v>30.027460280879101</v>
       </c>
       <c r="I38" s="7">
-        <v>268.03621599207497</v>
+        <v>270.81724488435299</v>
       </c>
       <c r="J38" s="12">
         <f t="shared" si="6"/>
-        <v>1764.9999999999982</v>
+        <v>1741.9999999999982</v>
       </c>
       <c r="K38" s="9">
         <f>G38/J38</f>
-        <v>0.54801998996346346</v>
+        <v>0.5323421902942348</v>
       </c>
       <c r="M38" s="4">
-        <v>0.37902058698336599</v>
+        <v>0.37382768003030098</v>
       </c>
       <c r="N38" s="2" t="s">
         <v>16</v>
@@ -5899,33 +5899,33 @@
         <v>9</v>
       </c>
       <c r="C39" s="7">
-        <v>5.8877996542020501</v>
+        <v>5.7548644567000302</v>
       </c>
       <c r="D39" s="7">
-        <v>2.6100242126392699</v>
+        <v>2.39159106502458</v>
       </c>
       <c r="E39" s="7">
-        <v>18.6314291833209</v>
+        <v>19.479628783800202</v>
       </c>
       <c r="F39" s="7">
-        <v>7.3428537784869699</v>
+        <v>7.8792427922115502</v>
       </c>
       <c r="G39" s="7">
-        <v>31.159056839939801</v>
+        <v>30.327544113036002</v>
       </c>
       <c r="H39" s="6">
-        <v>7.0692126924978496</v>
+        <v>7.6498246743481397</v>
       </c>
       <c r="I39" s="7">
-        <v>22.299623638912902</v>
+        <v>22.517304114879401</v>
       </c>
       <c r="J39" s="12">
         <f t="shared" si="6"/>
-        <v>94.99999999999973</v>
+        <v>95.999999999999915</v>
       </c>
       <c r="K39" s="9">
         <f>H39/J39</f>
-        <v>7.4412765184188101E-2</v>
+        <v>7.968567369112653E-2</v>
       </c>
     </row>
     <row r="40" spans="2:14" x14ac:dyDescent="0.35">
@@ -5933,33 +5933,33 @@
         <v>10</v>
       </c>
       <c r="C40" s="7">
-        <v>59.760706249268701</v>
+        <v>61.4204760327572</v>
       </c>
       <c r="D40" s="7">
-        <v>26.5293609196695</v>
+        <v>23.440360725882801</v>
       </c>
       <c r="E40" s="7">
-        <v>174.38720361534899</v>
+        <v>171.720863284545</v>
       </c>
       <c r="F40" s="7">
-        <v>58.086582224230597</v>
+        <v>62.5094538504922</v>
       </c>
       <c r="G40" s="7">
-        <v>275.61489663522798</v>
+        <v>268.79584293142699</v>
       </c>
       <c r="H40" s="7">
-        <v>22.2095085207702</v>
+        <v>22.889989387520799</v>
       </c>
       <c r="I40" s="6">
-        <v>320.41174183548401</v>
+        <v>320.22301378737399</v>
       </c>
       <c r="J40" s="12">
         <f t="shared" si="6"/>
-        <v>937</v>
+        <v>930.99999999999909</v>
       </c>
       <c r="K40" s="9">
         <f>I40/J40</f>
-        <v>0.34195490057148775</v>
+        <v>0.34395597614111095</v>
       </c>
     </row>
     <row r="41" spans="2:14" x14ac:dyDescent="0.35">
@@ -5968,35 +5968,35 @@
       </c>
       <c r="C41" s="8">
         <f>SUM(C34:C40)</f>
-        <v>278.37705033019165</v>
+        <v>290.2966206254136</v>
       </c>
       <c r="D41" s="8">
         <f t="shared" ref="D41:I41" si="7">SUM(D34:D40)</f>
-        <v>140.06319017993701</v>
+        <v>131.53276363201579</v>
       </c>
       <c r="E41" s="8">
         <f t="shared" si="7"/>
-        <v>802.20994190966417</v>
+        <v>818.0819251566395</v>
       </c>
       <c r="F41" s="8">
         <f t="shared" si="7"/>
-        <v>312.63638082842289</v>
+        <v>333.22798693142454</v>
       </c>
       <c r="G41" s="8">
         <f t="shared" si="7"/>
-        <v>1799.2914600589679</v>
+        <v>1748.9564878586318</v>
       </c>
       <c r="H41" s="8">
         <f t="shared" si="7"/>
-        <v>90.867044745056106</v>
+        <v>94.740664619243717</v>
       </c>
       <c r="I41" s="8">
         <f t="shared" si="7"/>
-        <v>920.55493194775659</v>
+        <v>927.16355117662579</v>
       </c>
       <c r="J41" s="12">
         <f>SUM(J34:J40)</f>
-        <v>4343.9999999999964</v>
+        <v>4343.9999999999945</v>
       </c>
       <c r="K41" s="10"/>
     </row>
@@ -6006,31 +6006,31 @@
       </c>
       <c r="C42" s="9">
         <f>C34/C41</f>
-        <v>0.28439646289792769</v>
+        <v>0.26168729952919229</v>
       </c>
       <c r="D42" s="9">
         <f>IFERROR(D35/D41, 0)</f>
-        <v>4.0975863080481928E-2</v>
+        <v>4.8007289660492912E-2</v>
       </c>
       <c r="E42" s="9">
         <f>IFERROR(E36/E41, 0)</f>
-        <v>0.22746926696772929</v>
+        <v>0.23099357278459279</v>
       </c>
       <c r="F42" s="9">
         <f>IFERROR(F37/F41, 0)</f>
-        <v>0.26977803034010023</v>
+        <v>0.292416528619871</v>
       </c>
       <c r="G42" s="9">
         <f>IFERROR(G38/G41, 0)</f>
-        <v>0.53757565339292623</v>
+        <v>0.53022479514511101</v>
       </c>
       <c r="H42" s="9">
         <f>IFERROR(H39/H41, 0)</f>
-        <v>7.779732148582362E-2</v>
+        <v>8.0744891384204071E-2</v>
       </c>
       <c r="I42" s="9">
         <f>IFERROR(I40/I41, 0)</f>
-        <v>0.34806368497482348</v>
+        <v>0.34537920885801854</v>
       </c>
       <c r="J42" s="10"/>
       <c r="K42" s="10"/>
@@ -6041,31 +6041,31 @@
       </c>
       <c r="C43" s="7">
         <f>C41-J34</f>
-        <v>-3.6229496698081789</v>
+        <v>27.296620625413709</v>
       </c>
       <c r="D43" s="7">
         <f>D41-J35</f>
-        <v>13.063190179937038</v>
+        <v>-20.467236367983872</v>
       </c>
       <c r="E43" s="7">
         <f>E41-J36</f>
-        <v>-18.790058090334696</v>
+        <v>-9.918074843358454</v>
       </c>
       <c r="F43" s="7">
         <f>F41-J37</f>
-        <v>-4.3636191715768859</v>
+        <v>1.2279869314246525</v>
       </c>
       <c r="G43" s="7">
         <f>G41-J38</f>
-        <v>34.291460058969733</v>
+        <v>6.9564878586336363</v>
       </c>
       <c r="H43" s="7">
         <f>H41-J39</f>
-        <v>-4.1329552549436244</v>
+        <v>-1.2593353807561982</v>
       </c>
       <c r="I43" s="7">
         <f>I41-J40</f>
-        <v>-16.445068052243414</v>
+        <v>-3.8364488233733027</v>
       </c>
       <c r="J43" s="10"/>
       <c r="K43" s="10"/>
@@ -6076,31 +6076,31 @@
       </c>
       <c r="C44" s="9">
         <f>C43/$J41</f>
-        <v>-8.3401235492821873E-4</v>
+        <v>6.2837524459976391E-3</v>
       </c>
       <c r="D44" s="9">
         <f t="shared" ref="D44:I44" si="8">D43/$J41</f>
-        <v>3.007180059838179E-3</v>
+        <v>-4.7116105819484111E-3</v>
       </c>
       <c r="E44" s="9">
         <f t="shared" si="8"/>
-        <v>-4.3255198182170149E-3</v>
+        <v>-2.2831664004048036E-3</v>
       </c>
       <c r="F44" s="9">
         <f t="shared" si="8"/>
-        <v>-1.0045163838804994E-3</v>
+        <v>2.8268575769444155E-4</v>
       </c>
       <c r="G44" s="9">
         <f t="shared" si="8"/>
-        <v>7.8939825181790421E-3</v>
+        <v>1.6014014407536015E-3</v>
       </c>
       <c r="H44" s="9">
         <f t="shared" si="8"/>
-        <v>-9.5141695555792539E-4</v>
+        <v>-2.8990225155529464E-4</v>
       </c>
       <c r="I44" s="9">
         <f t="shared" si="8"/>
-        <v>-3.7856970654335698E-3</v>
+        <v>-8.8316041053713339E-4</v>
       </c>
       <c r="J44" s="10"/>
       <c r="K44" s="10"/>
@@ -6116,7 +6116,7 @@
   <dimension ref="A2:N44"/>
   <sheetViews>
     <sheetView topLeftCell="B12" workbookViewId="0">
-      <selection activeCell="C34" activeCellId="2" sqref="C4:K14 C19:K29 C34:K44"/>
+      <selection activeCell="C34" sqref="C34:C40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -7089,37 +7089,37 @@
         <v>4</v>
       </c>
       <c r="C34" s="13">
-        <v>111</v>
+        <v>126</v>
       </c>
       <c r="D34" s="10">
         <v>0</v>
       </c>
       <c r="E34" s="10">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="F34" s="10">
         <v>2</v>
       </c>
       <c r="G34" s="10">
-        <v>99</v>
+        <v>83</v>
       </c>
       <c r="H34" s="10">
         <v>0</v>
       </c>
       <c r="I34" s="10">
-        <v>47</v>
+        <v>81</v>
       </c>
       <c r="J34" s="12">
         <f>SUM(C34:I34)</f>
-        <v>277</v>
+        <v>303</v>
       </c>
       <c r="K34" s="9">
         <f>C34/J34</f>
-        <v>0.4007220216606498</v>
+        <v>0.41584158415841582</v>
       </c>
       <c r="M34" s="3">
         <f>AVERAGE(K34:K40)</f>
-        <v>0.29493909728978052</v>
+        <v>0.3029264708424883</v>
       </c>
       <c r="N34" s="2" t="s">
         <v>12</v>
@@ -7130,29 +7130,29 @@
         <v>5</v>
       </c>
       <c r="C35" s="10">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="D35" s="13">
         <v>0</v>
       </c>
       <c r="E35" s="10">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F35" s="10">
         <v>6</v>
       </c>
       <c r="G35" s="10">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="H35" s="10">
         <v>0</v>
       </c>
       <c r="I35" s="10">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="J35" s="12">
         <f t="shared" ref="J35:J40" si="6">SUM(C35:I35)</f>
-        <v>145</v>
+        <v>125</v>
       </c>
       <c r="K35" s="9">
         <f>D35/J35</f>
@@ -7160,7 +7160,7 @@
       </c>
       <c r="M35" s="3">
         <f>AVERAGE(C42:I42)</f>
-        <v>0.39393590356714864</v>
+        <v>0.44240971340188473</v>
       </c>
       <c r="N35" s="2" t="s">
         <v>14</v>
@@ -7171,19 +7171,19 @@
         <v>6</v>
       </c>
       <c r="C36" s="10">
-        <v>67</v>
+        <v>56</v>
       </c>
       <c r="D36" s="10">
         <v>0</v>
       </c>
       <c r="E36" s="13">
-        <v>86</v>
+        <v>70</v>
       </c>
       <c r="F36" s="10">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="G36" s="10">
-        <v>464</v>
+        <v>492</v>
       </c>
       <c r="H36" s="10">
         <v>0</v>
@@ -7193,15 +7193,15 @@
       </c>
       <c r="J36" s="12">
         <f t="shared" si="6"/>
-        <v>839</v>
+        <v>833</v>
       </c>
       <c r="K36" s="9">
         <f>E36/J36</f>
-        <v>0.10250297973778308</v>
+        <v>8.4033613445378158E-2</v>
       </c>
       <c r="M36" s="4">
         <f>2*M34*M35/(M34+M35)</f>
-        <v>0.33732418695292293</v>
+        <v>0.35961654882792954</v>
       </c>
       <c r="N36" s="2" t="s">
         <v>15</v>
@@ -7218,31 +7218,31 @@
         <v>0</v>
       </c>
       <c r="E37" s="10">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="F37" s="13">
-        <v>118</v>
+        <v>94</v>
       </c>
       <c r="G37" s="10">
-        <v>124</v>
+        <v>147</v>
       </c>
       <c r="H37" s="10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I37" s="10">
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="J37" s="12">
         <f t="shared" si="6"/>
-        <v>323</v>
+        <v>305</v>
       </c>
       <c r="K37" s="9">
         <f>F37/J37</f>
-        <v>0.3653250773993808</v>
+        <v>0.30819672131147541</v>
       </c>
       <c r="M37" s="4">
         <f>SUM(C34,D35,E36,F37,G38,H39,I40)/J41</f>
-        <v>0.4677716390423573</v>
+        <v>0.48388581952117865</v>
       </c>
       <c r="N37" s="2" t="s">
         <v>13</v>
@@ -7253,36 +7253,36 @@
         <v>8</v>
       </c>
       <c r="C38" s="10">
-        <v>72</v>
+        <v>60</v>
       </c>
       <c r="D38" s="10">
         <v>0</v>
       </c>
       <c r="E38" s="10">
-        <v>86</v>
+        <v>65</v>
       </c>
       <c r="F38" s="10">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="G38" s="13">
-        <v>1359</v>
+        <v>1418</v>
       </c>
       <c r="H38" s="10">
         <v>0</v>
       </c>
       <c r="I38" s="10">
-        <v>194</v>
+        <v>166</v>
       </c>
       <c r="J38" s="12">
         <f t="shared" si="6"/>
-        <v>1770</v>
+        <v>1761</v>
       </c>
       <c r="K38" s="9">
         <f>G38/J38</f>
-        <v>0.76779661016949152</v>
+        <v>0.80522430437251558</v>
       </c>
       <c r="M38" s="4">
-        <v>0.36863659867827497</v>
+        <v>0.37497864554075899</v>
       </c>
       <c r="N38" s="2" t="s">
         <v>16</v>
@@ -7299,27 +7299,27 @@
         <v>0</v>
       </c>
       <c r="E39" s="10">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="F39" s="10">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G39" s="10">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="H39" s="13">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="I39" s="10">
         <v>20</v>
       </c>
       <c r="J39" s="12">
         <f t="shared" si="6"/>
-        <v>95</v>
+        <v>107</v>
       </c>
       <c r="K39" s="9">
         <f>H39/J39</f>
-        <v>3.1578947368421054E-2</v>
+        <v>8.4112149532710276E-2</v>
       </c>
     </row>
     <row r="40" spans="2:14" x14ac:dyDescent="0.35">
@@ -7333,27 +7333,27 @@
         <v>0</v>
       </c>
       <c r="E40" s="10">
-        <v>56</v>
+        <v>34</v>
       </c>
       <c r="F40" s="10">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="G40" s="10">
-        <v>396</v>
+        <v>407</v>
       </c>
       <c r="H40" s="10">
         <v>0</v>
       </c>
       <c r="I40" s="13">
-        <v>355</v>
+        <v>385</v>
       </c>
       <c r="J40" s="12">
         <f t="shared" si="6"/>
-        <v>895</v>
+        <v>910</v>
       </c>
       <c r="K40" s="9">
         <f>I40/J40</f>
-        <v>0.39664804469273746</v>
+        <v>0.42307692307692307</v>
       </c>
     </row>
     <row r="41" spans="2:14" x14ac:dyDescent="0.35">
@@ -7362,7 +7362,7 @@
       </c>
       <c r="C41" s="12">
         <f>SUM(C34:C40)</f>
-        <v>322</v>
+        <v>304</v>
       </c>
       <c r="D41" s="12">
         <f t="shared" ref="D41:I41" si="7">SUM(D34:D40)</f>
@@ -7370,23 +7370,23 @@
       </c>
       <c r="E41" s="12">
         <f t="shared" si="7"/>
-        <v>301</v>
+        <v>231</v>
       </c>
       <c r="F41" s="12">
         <f t="shared" si="7"/>
-        <v>270</v>
+        <v>227</v>
       </c>
       <c r="G41" s="12">
         <f t="shared" si="7"/>
-        <v>2594</v>
+        <v>2697</v>
       </c>
       <c r="H41" s="12">
         <f t="shared" si="7"/>
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="I41" s="12">
         <f t="shared" si="7"/>
-        <v>853</v>
+        <v>876</v>
       </c>
       <c r="J41" s="12">
         <f>SUM(J34:J40)</f>
@@ -7400,7 +7400,7 @@
       </c>
       <c r="C42" s="9">
         <f>C34/C41</f>
-        <v>0.34472049689440992</v>
+        <v>0.41447368421052633</v>
       </c>
       <c r="D42" s="9">
         <f>IFERROR(D35/D41, 0)</f>
@@ -7408,23 +7408,23 @@
       </c>
       <c r="E42" s="9">
         <f>IFERROR(E36/E41, 0)</f>
-        <v>0.2857142857142857</v>
+        <v>0.30303030303030304</v>
       </c>
       <c r="F42" s="9">
         <f>IFERROR(F37/F41, 0)</f>
-        <v>0.43703703703703706</v>
+        <v>0.41409691629955947</v>
       </c>
       <c r="G42" s="9">
         <f>IFERROR(G38/G41, 0)</f>
-        <v>0.52390131071703927</v>
+        <v>0.52576937337782725</v>
       </c>
       <c r="H42" s="9">
         <f>IFERROR(H39/H41, 0)</f>
-        <v>0.75</v>
+        <v>1</v>
       </c>
       <c r="I42" s="9">
         <f>IFERROR(I40/I41, 0)</f>
-        <v>0.41617819460726846</v>
+        <v>0.43949771689497719</v>
       </c>
       <c r="J42" s="10"/>
       <c r="K42" s="10"/>
@@ -7435,31 +7435,31 @@
       </c>
       <c r="C43" s="10">
         <f>C41-J34</f>
-        <v>45</v>
+        <v>1</v>
       </c>
       <c r="D43" s="10">
         <f>D41-J35</f>
-        <v>-145</v>
+        <v>-125</v>
       </c>
       <c r="E43" s="10">
         <f>E41-J36</f>
-        <v>-538</v>
+        <v>-602</v>
       </c>
       <c r="F43" s="10">
         <f>F41-J37</f>
-        <v>-53</v>
+        <v>-78</v>
       </c>
       <c r="G43" s="10">
         <f>G41-J38</f>
-        <v>824</v>
+        <v>936</v>
       </c>
       <c r="H43" s="10">
         <f>H41-J39</f>
-        <v>-91</v>
+        <v>-98</v>
       </c>
       <c r="I43" s="10">
         <f>I41-J40</f>
-        <v>-42</v>
+        <v>-34</v>
       </c>
       <c r="J43" s="10"/>
       <c r="K43" s="10"/>
@@ -7470,31 +7470,31 @@
       </c>
       <c r="C44" s="9">
         <f>C43/$J41</f>
-        <v>1.0359116022099447E-2</v>
+        <v>2.3020257826887662E-4</v>
       </c>
       <c r="D44" s="9">
         <f t="shared" ref="D44:I44" si="8">D43/$J41</f>
-        <v>-3.3379373848987107E-2</v>
+        <v>-2.8775322283609576E-2</v>
       </c>
       <c r="E44" s="9">
         <f t="shared" si="8"/>
-        <v>-0.12384898710865562</v>
+        <v>-0.13858195211786373</v>
       </c>
       <c r="F44" s="9">
         <f t="shared" si="8"/>
-        <v>-1.220073664825046E-2</v>
+        <v>-1.7955801104972375E-2</v>
       </c>
       <c r="G44" s="9">
         <f t="shared" si="8"/>
-        <v>0.18968692449355432</v>
+        <v>0.21546961325966851</v>
       </c>
       <c r="H44" s="9">
         <f t="shared" si="8"/>
-        <v>-2.094843462246777E-2</v>
+        <v>-2.2559852670349909E-2</v>
       </c>
       <c r="I44" s="9">
         <f t="shared" si="8"/>
-        <v>-9.6685082872928173E-3</v>
+        <v>-7.8268876611418056E-3</v>
       </c>
       <c r="J44" s="10"/>
       <c r="K44" s="10"/>
@@ -7509,8 +7509,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E829243F-C70A-488C-9BB1-F13AC3A1858F}">
   <dimension ref="A2:N44"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3:I3"/>
+    <sheetView topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="C34" sqref="C34:C40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -8483,37 +8483,37 @@
         <v>4</v>
       </c>
       <c r="C34" s="6">
-        <v>74.784847119178707</v>
+        <v>87.676129606414904</v>
       </c>
       <c r="D34" s="7">
-        <v>6.3506508979974603</v>
+        <v>7.1830320383052504</v>
       </c>
       <c r="E34" s="7">
-        <v>51.678621874917901</v>
+        <v>57.856960491566802</v>
       </c>
       <c r="F34" s="7">
-        <v>5.9813978379665098</v>
+        <v>6.2176999570996996</v>
       </c>
       <c r="G34" s="7">
-        <v>75.762781955465798</v>
+        <v>74.789578805618603</v>
       </c>
       <c r="H34" s="7">
-        <v>5.6397393542954202</v>
+        <v>5.2819167351076102</v>
       </c>
       <c r="I34" s="7">
-        <v>56.801960960178</v>
+        <v>63.994682365887002</v>
       </c>
       <c r="J34" s="12">
         <f>SUM(C34:I34)</f>
-        <v>276.99999999999977</v>
+        <v>302.99999999999989</v>
       </c>
       <c r="K34" s="9">
         <f>C34/J34</f>
-        <v>0.26998139754216161</v>
+        <v>0.28936016371754103</v>
       </c>
       <c r="M34" s="3">
         <f>AVERAGE(K34:K40)</f>
-        <v>0.24591235027290997</v>
+        <v>0.25365328154956518</v>
       </c>
       <c r="N34" s="2" t="s">
         <v>12</v>
@@ -8524,37 +8524,37 @@
         <v>5</v>
       </c>
       <c r="C35" s="7">
-        <v>8.6085737226375603</v>
+        <v>5.9659866656521601</v>
       </c>
       <c r="D35" s="6">
-        <v>5.40836053206879</v>
+        <v>5.3779450571804697</v>
       </c>
       <c r="E35" s="7">
-        <v>27.756152482647099</v>
+        <v>25.753533676457799</v>
       </c>
       <c r="F35" s="7">
-        <v>8.8491194859863196</v>
+        <v>8.4144171774376399</v>
       </c>
       <c r="G35" s="7">
-        <v>64.000055559633793</v>
+        <v>53.221518511841403</v>
       </c>
       <c r="H35" s="7">
-        <v>2.7709651402308002</v>
+        <v>2.3114258389244702</v>
       </c>
       <c r="I35" s="7">
-        <v>27.606773076795498</v>
+        <v>23.9551730725059</v>
       </c>
       <c r="J35" s="12">
         <f t="shared" ref="J35:J40" si="6">SUM(C35:I35)</f>
-        <v>144.99999999999986</v>
+        <v>124.99999999999984</v>
       </c>
       <c r="K35" s="9">
         <f>D35/J35</f>
-        <v>3.7299038152198587E-2</v>
+        <v>4.3023560457443814E-2</v>
       </c>
       <c r="M35" s="3">
         <f>AVERAGE(C42:I42)</f>
-        <v>0.24502141351349596</v>
+        <v>0.25501800751293419</v>
       </c>
       <c r="N35" s="2" t="s">
         <v>14</v>
@@ -8565,37 +8565,37 @@
         <v>6</v>
       </c>
       <c r="C36" s="7">
-        <v>58.681284351141699</v>
+        <v>51.981568930459801</v>
       </c>
       <c r="D36" s="7">
-        <v>28.208201103046299</v>
+        <v>29.995102833539399</v>
       </c>
       <c r="E36" s="6">
-        <v>184.855670678856</v>
+        <v>191.17040517057299</v>
       </c>
       <c r="F36" s="7">
-        <v>60.938194783822802</v>
+        <v>64.781148783936999</v>
       </c>
       <c r="G36" s="7">
-        <v>307.02059201533302</v>
+        <v>300.785007352962</v>
       </c>
       <c r="H36" s="7">
-        <v>18.537471511694701</v>
+        <v>18.0677820050173</v>
       </c>
       <c r="I36" s="7">
-        <v>180.75858555610299</v>
+        <v>176.21898492350999</v>
       </c>
       <c r="J36" s="12">
         <f t="shared" si="6"/>
-        <v>838.9999999999975</v>
+        <v>832.99999999999852</v>
       </c>
       <c r="K36" s="9">
         <f>E36/J36</f>
-        <v>0.22032857053498994</v>
+        <v>0.22949628471857542</v>
       </c>
       <c r="M36" s="4">
         <f>2*M34*M35/(M34+M35)</f>
-        <v>0.24546607346611174</v>
+        <v>0.25433381380382797</v>
       </c>
       <c r="N36" s="2" t="s">
         <v>15</v>
@@ -8606,37 +8606,37 @@
         <v>7</v>
       </c>
       <c r="C37" s="7">
-        <v>6.3842587936069899</v>
+        <v>4.9706974257046799</v>
       </c>
       <c r="D37" s="7">
-        <v>8.7483643407856206</v>
+        <v>8.5468242637111604</v>
       </c>
       <c r="E37" s="7">
-        <v>62.806484517941897</v>
+        <v>58.646991254138399</v>
       </c>
       <c r="F37" s="6">
-        <v>88.409247361241199</v>
+        <v>84.755351101521299</v>
       </c>
       <c r="G37" s="7">
-        <v>88.216159527984502</v>
+        <v>84.202265965243001</v>
       </c>
       <c r="H37" s="7">
-        <v>8.1723982762364695</v>
+        <v>7.2085607190598102</v>
       </c>
       <c r="I37" s="7">
-        <v>60.2630871822033</v>
+        <v>56.669309270621497</v>
       </c>
       <c r="J37" s="12">
         <f t="shared" si="6"/>
-        <v>323</v>
+        <v>304.99999999999983</v>
       </c>
       <c r="K37" s="9">
         <f>F37/J37</f>
-        <v>0.27371284012768171</v>
+        <v>0.27788639705416834</v>
       </c>
       <c r="M37" s="4">
         <f>SUM(C34,D35,E36,F37,G38,H39,I40)/J41</f>
-        <v>0.3686365986782752</v>
+        <v>0.37497864554075944</v>
       </c>
       <c r="N37" s="2" t="s">
         <v>13</v>
@@ -8647,36 +8647,36 @@
         <v>8</v>
       </c>
       <c r="C38" s="7">
-        <v>71.885525615483601</v>
+        <v>71.686849420315497</v>
       </c>
       <c r="D38" s="7">
-        <v>58.0345101244164</v>
+        <v>63.173372593245702</v>
       </c>
       <c r="E38" s="7">
-        <v>292.56138092674701</v>
+        <v>291.17289095693798</v>
       </c>
       <c r="F38" s="7">
-        <v>95.648975915264103</v>
+        <v>92.257370009281104</v>
       </c>
       <c r="G38" s="6">
-        <v>943.03850915650298</v>
+        <v>945.39631894507795</v>
       </c>
       <c r="H38" s="7">
-        <v>30.0198008897599</v>
+        <v>28.752265968622201</v>
       </c>
       <c r="I38" s="7">
-        <v>278.81129737181902</v>
+        <v>268.56093210651699</v>
       </c>
       <c r="J38" s="12">
         <f t="shared" si="6"/>
-        <v>1769.9999999999932</v>
+        <v>1760.9999999999973</v>
       </c>
       <c r="K38" s="9">
         <f>G38/J38</f>
-        <v>0.53279011816751787</v>
+        <v>0.53685196987227679</v>
       </c>
       <c r="M38" s="4">
-        <v>0.36863659867827497</v>
+        <v>0.37497864554075899</v>
       </c>
       <c r="N38" s="2" t="s">
         <v>16</v>
@@ -8687,33 +8687,33 @@
         <v>9</v>
       </c>
       <c r="C39" s="7">
-        <v>4.2599734504665197</v>
+        <v>5.3903411134396304</v>
       </c>
       <c r="D39" s="7">
-        <v>2.7198462725591499</v>
+        <v>3.04961854302254</v>
       </c>
       <c r="E39" s="7">
-        <v>19.662356466278901</v>
+        <v>21.371810838568098</v>
       </c>
       <c r="F39" s="7">
-        <v>8.1110327546541399</v>
+        <v>9.0465201096968606</v>
       </c>
       <c r="G39" s="7">
-        <v>33.0537597262825</v>
+        <v>36.3051799069775</v>
       </c>
       <c r="H39" s="6">
-        <v>4.9578025724683101</v>
+        <v>6.4649846556751598</v>
       </c>
       <c r="I39" s="7">
-        <v>22.235228757290301</v>
+        <v>25.37154483262</v>
       </c>
       <c r="J39" s="12">
         <f t="shared" si="6"/>
-        <v>94.999999999999829</v>
+        <v>106.9999999999998</v>
       </c>
       <c r="K39" s="9">
         <f>H39/J39</f>
-        <v>5.2187395499666514E-2</v>
+        <v>6.0420417342758617E-2</v>
       </c>
     </row>
     <row r="40" spans="2:14" x14ac:dyDescent="0.35">
@@ -8721,33 +8721,33 @@
         <v>10</v>
       </c>
       <c r="C40" s="7">
-        <v>54.7528940385399</v>
+        <v>53.981623684672101</v>
       </c>
       <c r="D40" s="7">
-        <v>22.197217397888199</v>
+        <v>24.8413459537154</v>
       </c>
       <c r="E40" s="7">
-        <v>164.228302401246</v>
+        <v>168.18973928035101</v>
       </c>
       <c r="F40" s="7">
-        <v>59.343730346236804</v>
+        <v>59.574089672892399</v>
       </c>
       <c r="G40" s="7">
-        <v>272.27351604483903</v>
+        <v>273.65077001028902</v>
       </c>
       <c r="H40" s="7">
-        <v>22.301392533141001</v>
+        <v>21.696329705464201</v>
       </c>
       <c r="I40" s="6">
-        <v>299.902947238107</v>
+        <v>308.06610169261398</v>
       </c>
       <c r="J40" s="12">
         <f t="shared" si="6"/>
-        <v>894.99999999999795</v>
+        <v>909.99999999999818</v>
       </c>
       <c r="K40" s="9">
         <f>I40/J40</f>
-        <v>0.33508709188615382</v>
+        <v>0.33853417768419186</v>
       </c>
     </row>
     <row r="41" spans="2:14" x14ac:dyDescent="0.35">
@@ -8756,35 +8756,35 @@
       </c>
       <c r="C41" s="8">
         <f>SUM(C34:C40)</f>
-        <v>279.35735709105501</v>
+        <v>281.65319684665877</v>
       </c>
       <c r="D41" s="8">
         <f t="shared" ref="D41:I41" si="7">SUM(D34:D40)</f>
-        <v>131.66715066876193</v>
+        <v>142.16724128271991</v>
       </c>
       <c r="E41" s="8">
         <f t="shared" si="7"/>
-        <v>803.54896934863484</v>
+        <v>814.16233166859297</v>
       </c>
       <c r="F41" s="8">
         <f t="shared" si="7"/>
-        <v>327.28169848517189</v>
+        <v>325.04659681186598</v>
       </c>
       <c r="G41" s="8">
         <f t="shared" si="7"/>
-        <v>1783.3653739860415</v>
+        <v>1768.3506394980095</v>
       </c>
       <c r="H41" s="8">
         <f t="shared" si="7"/>
-        <v>92.399570277826598</v>
+        <v>89.783265627870747</v>
       </c>
       <c r="I41" s="8">
         <f t="shared" si="7"/>
-        <v>926.37988014249618</v>
+        <v>922.83672826427528</v>
       </c>
       <c r="J41" s="12">
         <f>SUM(J34:J40)</f>
-        <v>4343.9999999999882</v>
+        <v>4343.9999999999936</v>
       </c>
       <c r="K41" s="10"/>
     </row>
@@ -8794,31 +8794,31 @@
       </c>
       <c r="C42" s="9">
         <f>C34/C41</f>
-        <v>0.2677031594868754</v>
+        <v>0.31129108630053526</v>
       </c>
       <c r="D42" s="9">
         <f>IFERROR(D35/D41, 0)</f>
-        <v>4.1076004945794921E-2</v>
+        <v>3.7828300026485399E-2</v>
       </c>
       <c r="E42" s="9">
         <f>IFERROR(E36/E41, 0)</f>
-        <v>0.2300490420997017</v>
+        <v>0.23480625144960579</v>
       </c>
       <c r="F42" s="9">
         <f>IFERROR(F37/F41, 0)</f>
-        <v>0.27013196206950979</v>
+        <v>0.26074831095855749</v>
       </c>
       <c r="G42" s="9">
         <f>IFERROR(G38/G41, 0)</f>
-        <v>0.52879713989775168</v>
+        <v>0.53462039588113153</v>
       </c>
       <c r="H42" s="9">
         <f>IFERROR(H39/H41, 0)</f>
-        <v>5.365612153347913E-2</v>
+        <v>7.2006566150878373E-2</v>
       </c>
       <c r="I42" s="9">
         <f>IFERROR(I40/I41, 0)</f>
-        <v>0.32373646456135879</v>
+        <v>0.33382514182334566</v>
       </c>
       <c r="J42" s="10"/>
       <c r="K42" s="10"/>
@@ -8829,31 +8829,31 @@
       </c>
       <c r="C43" s="7">
         <f>C41-J34</f>
-        <v>2.3573570910552348</v>
+        <v>-21.346803153341114</v>
       </c>
       <c r="D43" s="7">
         <f>D41-J35</f>
-        <v>-13.332849331237924</v>
+        <v>17.16724128272007</v>
       </c>
       <c r="E43" s="7">
         <f>E41-J36</f>
-        <v>-35.451030651362657</v>
+        <v>-18.837668331405553</v>
       </c>
       <c r="F43" s="7">
         <f>F41-J37</f>
-        <v>4.2816984851718871</v>
+        <v>20.046596811866152</v>
       </c>
       <c r="G43" s="7">
         <f>G41-J38</f>
-        <v>13.365373986048326</v>
+        <v>7.3506394980122423</v>
       </c>
       <c r="H43" s="7">
         <f>H41-J39</f>
-        <v>-2.6004297221732315</v>
+        <v>-17.216734372129054</v>
       </c>
       <c r="I43" s="7">
         <f>I41-J40</f>
-        <v>31.379880142498223</v>
+        <v>12.836728264277099</v>
       </c>
       <c r="J43" s="10"/>
       <c r="K43" s="10"/>
@@ -8864,31 +8864,31 @@
       </c>
       <c r="C44" s="9">
         <f>C43/$J41</f>
-        <v>5.4266968026133551E-4</v>
+        <v>-4.9140891236973171E-3</v>
       </c>
       <c r="D44" s="9">
         <f t="shared" ref="D44:I44" si="8">D43/$J41</f>
-        <v>-3.0692562917214459E-3</v>
+        <v>3.9519432050460629E-3</v>
       </c>
       <c r="E44" s="9">
         <f t="shared" si="8"/>
-        <v>-8.1609186582326781E-3</v>
+        <v>-4.3364798184635312E-3</v>
       </c>
       <c r="F44" s="9">
         <f t="shared" si="8"/>
-        <v>9.8565803065651437E-4</v>
+        <v>4.6147782716082367E-3</v>
       </c>
       <c r="G44" s="9">
         <f t="shared" si="8"/>
-        <v>3.0767435511161053E-3</v>
+        <v>1.6921361643674616E-3</v>
       </c>
       <c r="H44" s="9">
         <f t="shared" si="8"/>
-        <v>-5.98625626651298E-4</v>
+        <v>-3.9633366418345027E-3</v>
       </c>
       <c r="I44" s="9">
         <f t="shared" si="8"/>
-        <v>7.2237293145714339E-3</v>
+        <v>2.955047942973554E-3</v>
       </c>
       <c r="J44" s="10"/>
       <c r="K44" s="10"/>
@@ -8904,7 +8904,7 @@
   <dimension ref="A2:N44"/>
   <sheetViews>
     <sheetView topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="C33" sqref="C33:I33"/>
+      <selection activeCell="C34" sqref="C34:C40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -9883,31 +9883,31 @@
         <v>0</v>
       </c>
       <c r="E34" s="10">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="F34" s="10">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G34" s="10">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="H34" s="10">
         <v>0</v>
       </c>
       <c r="I34" s="10">
-        <v>46</v>
+        <v>69</v>
       </c>
       <c r="J34" s="12">
         <f>SUM(C34:I34)</f>
-        <v>268</v>
+        <v>302</v>
       </c>
       <c r="K34" s="9">
         <f>C34/J34</f>
-        <v>0.48507462686567165</v>
+        <v>0.43046357615894038</v>
       </c>
       <c r="M34" s="3">
         <f>AVERAGE(K34:K40)</f>
-        <v>0.32265929315065672</v>
+        <v>0.31721146828922508</v>
       </c>
       <c r="N34" s="2" t="s">
         <v>12</v>
@@ -9918,29 +9918,29 @@
         <v>5</v>
       </c>
       <c r="C35" s="10">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="D35" s="13">
         <v>0</v>
       </c>
       <c r="E35" s="10">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="F35" s="10">
         <v>5</v>
       </c>
       <c r="G35" s="10">
-        <v>82</v>
+        <v>94</v>
       </c>
       <c r="H35" s="10">
         <v>0</v>
       </c>
       <c r="I35" s="10">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="J35" s="12">
         <f t="shared" ref="J35:J40" si="6">SUM(C35:I35)</f>
-        <v>130</v>
+        <v>138</v>
       </c>
       <c r="K35" s="9">
         <f>D35/J35</f>
@@ -9948,7 +9948,7 @@
       </c>
       <c r="M35" s="3">
         <f>AVERAGE(C42:I42)</f>
-        <v>0.45310134664445606</v>
+        <v>0.43853478795409739</v>
       </c>
       <c r="N35" s="2" t="s">
         <v>14</v>
@@ -9959,37 +9959,37 @@
         <v>6</v>
       </c>
       <c r="C36" s="10">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="D36" s="10">
         <v>0</v>
       </c>
       <c r="E36" s="13">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F36" s="10">
         <v>53</v>
       </c>
       <c r="G36" s="10">
-        <v>437</v>
+        <v>427</v>
       </c>
       <c r="H36" s="10">
         <v>0</v>
       </c>
       <c r="I36" s="10">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="J36" s="12">
         <f t="shared" si="6"/>
-        <v>843</v>
+        <v>823</v>
       </c>
       <c r="K36" s="9">
         <f>E36/J36</f>
-        <v>0.11269276393831554</v>
+        <v>0.11421628189550426</v>
       </c>
       <c r="M36" s="4">
         <f>2*M34*M35/(M34+M35)</f>
-        <v>0.37691358064395553</v>
+        <v>0.36813484111533723</v>
       </c>
       <c r="N36" s="2" t="s">
         <v>15</v>
@@ -10000,37 +10000,37 @@
         <v>7</v>
       </c>
       <c r="C37" s="10">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D37" s="10">
         <v>0</v>
       </c>
       <c r="E37" s="10">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="F37" s="13">
-        <v>115</v>
+        <v>126</v>
       </c>
       <c r="G37" s="10">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="H37" s="10">
         <v>0</v>
       </c>
       <c r="I37" s="10">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="J37" s="12">
         <f t="shared" si="6"/>
-        <v>331</v>
+        <v>339</v>
       </c>
       <c r="K37" s="9">
         <f>F37/J37</f>
-        <v>0.34743202416918428</v>
+        <v>0.37168141592920356</v>
       </c>
       <c r="M37" s="4">
         <f>SUM(C34,D35,E36,F37,G38,H39,I40)/J41</f>
-        <v>0.48641804788213627</v>
+        <v>0.48020257826887663</v>
       </c>
       <c r="N37" s="2" t="s">
         <v>13</v>
@@ -10041,36 +10041,36 @@
         <v>8</v>
       </c>
       <c r="C38" s="10">
-        <v>71</v>
+        <v>57</v>
       </c>
       <c r="D38" s="10">
         <v>0</v>
       </c>
       <c r="E38" s="10">
-        <v>62</v>
+        <v>69</v>
       </c>
       <c r="F38" s="10">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G38" s="13">
-        <v>1328</v>
+        <v>1309</v>
       </c>
       <c r="H38" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I38" s="10">
         <v>207</v>
       </c>
       <c r="J38" s="12">
         <f t="shared" si="6"/>
-        <v>1722</v>
+        <v>1696</v>
       </c>
       <c r="K38" s="9">
         <f>G38/J38</f>
-        <v>0.77119628339140534</v>
+        <v>0.77181603773584906</v>
       </c>
       <c r="M38" s="4">
-        <v>0.37630594820937302</v>
+        <v>0.37719845395622598</v>
       </c>
       <c r="N38" s="2" t="s">
         <v>16</v>
@@ -10081,7 +10081,7 @@
         <v>9</v>
       </c>
       <c r="C39" s="10">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="D39" s="10">
         <v>0</v>
@@ -10093,21 +10093,21 @@
         <v>9</v>
       </c>
       <c r="G39" s="10">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="H39" s="13">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="I39" s="10">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="J39" s="12">
         <f t="shared" si="6"/>
-        <v>94</v>
+        <v>99</v>
       </c>
       <c r="K39" s="9">
         <f>H39/J39</f>
-        <v>8.5106382978723402E-2</v>
+        <v>9.0909090909090912E-2</v>
       </c>
     </row>
     <row r="40" spans="2:14" x14ac:dyDescent="0.35">
@@ -10115,33 +10115,33 @@
         <v>10</v>
       </c>
       <c r="C40" s="10">
-        <v>61</v>
+        <v>51</v>
       </c>
       <c r="D40" s="10">
         <v>0</v>
       </c>
       <c r="E40" s="10">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="F40" s="10">
         <v>49</v>
       </c>
       <c r="G40" s="10">
-        <v>374</v>
+        <v>389</v>
       </c>
       <c r="H40" s="10">
         <v>0</v>
       </c>
       <c r="I40" s="13">
-        <v>437</v>
+        <v>418</v>
       </c>
       <c r="J40" s="12">
         <f t="shared" si="6"/>
-        <v>956</v>
+        <v>947</v>
       </c>
       <c r="K40" s="9">
         <f>I40/J40</f>
-        <v>0.45711297071129708</v>
+        <v>0.44139387539598735</v>
       </c>
     </row>
     <row r="41" spans="2:14" x14ac:dyDescent="0.35">
@@ -10150,7 +10150,7 @@
       </c>
       <c r="C41" s="12">
         <f>SUM(C34:C40)</f>
-        <v>338</v>
+        <v>309</v>
       </c>
       <c r="D41" s="12">
         <f t="shared" ref="D41:I41" si="7">SUM(D34:D40)</f>
@@ -10158,23 +10158,23 @@
       </c>
       <c r="E41" s="12">
         <f t="shared" si="7"/>
-        <v>235</v>
+        <v>253</v>
       </c>
       <c r="F41" s="12">
         <f t="shared" si="7"/>
-        <v>286</v>
+        <v>297</v>
       </c>
       <c r="G41" s="12">
         <f t="shared" si="7"/>
-        <v>2509</v>
+        <v>2504</v>
       </c>
       <c r="H41" s="12">
         <f t="shared" si="7"/>
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="I41" s="12">
         <f t="shared" si="7"/>
-        <v>968</v>
+        <v>971</v>
       </c>
       <c r="J41" s="12">
         <f>SUM(J34:J40)</f>
@@ -10188,7 +10188,7 @@
       </c>
       <c r="C42" s="9">
         <f>C34/C41</f>
-        <v>0.38461538461538464</v>
+        <v>0.42071197411003236</v>
       </c>
       <c r="D42" s="9">
         <f>IFERROR(D35/D41, 0)</f>
@@ -10196,23 +10196,23 @@
       </c>
       <c r="E42" s="9">
         <f>IFERROR(E36/E41, 0)</f>
-        <v>0.40425531914893614</v>
+        <v>0.3715415019762846</v>
       </c>
       <c r="F42" s="9">
         <f>IFERROR(F37/F41, 0)</f>
-        <v>0.40209790209790208</v>
+        <v>0.42424242424242425</v>
       </c>
       <c r="G42" s="9">
         <f>IFERROR(G38/G41, 0)</f>
-        <v>0.52929453965723394</v>
+        <v>0.52276357827476039</v>
       </c>
       <c r="H42" s="9">
         <f>IFERROR(H39/H41, 0)</f>
-        <v>1</v>
+        <v>0.9</v>
       </c>
       <c r="I42" s="9">
         <f>IFERROR(I40/I41, 0)</f>
-        <v>0.45144628099173556</v>
+        <v>0.43048403707518024</v>
       </c>
       <c r="J42" s="10"/>
       <c r="K42" s="10"/>
@@ -10223,31 +10223,31 @@
       </c>
       <c r="C43" s="10">
         <f>C41-J34</f>
-        <v>70</v>
+        <v>7</v>
       </c>
       <c r="D43" s="10">
         <f>D41-J35</f>
-        <v>-130</v>
+        <v>-138</v>
       </c>
       <c r="E43" s="10">
         <f>E41-J36</f>
-        <v>-608</v>
+        <v>-570</v>
       </c>
       <c r="F43" s="10">
         <f>F41-J37</f>
-        <v>-45</v>
+        <v>-42</v>
       </c>
       <c r="G43" s="10">
         <f>G41-J38</f>
-        <v>787</v>
+        <v>808</v>
       </c>
       <c r="H43" s="10">
         <f>H41-J39</f>
-        <v>-86</v>
+        <v>-89</v>
       </c>
       <c r="I43" s="10">
         <f>I41-J40</f>
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="J43" s="10"/>
       <c r="K43" s="10"/>
@@ -10258,31 +10258,31 @@
       </c>
       <c r="C44" s="9">
         <f>C43/$J41</f>
-        <v>1.6114180478821363E-2</v>
+        <v>1.6114180478821363E-3</v>
       </c>
       <c r="D44" s="9">
         <f t="shared" ref="D44:I44" si="8">D43/$J41</f>
-        <v>-2.9926335174953959E-2</v>
+        <v>-3.1767955801104975E-2</v>
       </c>
       <c r="E44" s="9">
         <f t="shared" si="8"/>
-        <v>-0.13996316758747698</v>
+        <v>-0.13121546961325967</v>
       </c>
       <c r="F44" s="9">
         <f t="shared" si="8"/>
-        <v>-1.0359116022099447E-2</v>
+        <v>-9.6685082872928173E-3</v>
       </c>
       <c r="G44" s="9">
         <f t="shared" si="8"/>
-        <v>0.18116942909760589</v>
+        <v>0.1860036832412523</v>
       </c>
       <c r="H44" s="9">
         <f t="shared" si="8"/>
-        <v>-1.979742173112339E-2</v>
+        <v>-2.0488029465930018E-2</v>
       </c>
       <c r="I44" s="9">
         <f t="shared" si="8"/>
-        <v>2.7624309392265192E-3</v>
+        <v>5.5248618784530384E-3</v>
       </c>
       <c r="J44" s="10"/>
       <c r="K44" s="10"/>
@@ -10297,8 +10297,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DCF5E33F-F6FC-4E38-B0F5-D47375931366}">
   <dimension ref="A2:N44"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C33" sqref="C33:I33"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="L42" sqref="L42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -11271,37 +11271,37 @@
         <v>4</v>
       </c>
       <c r="C34" s="6">
-        <v>81.771043420555202</v>
+        <v>93.131354879246302</v>
       </c>
       <c r="D34" s="7">
-        <v>6.3733698699370001</v>
+        <v>6.6510506285737998</v>
       </c>
       <c r="E34" s="7">
-        <v>50.991134563976502</v>
+        <v>54.777011663961197</v>
       </c>
       <c r="F34" s="7">
-        <v>4.2567042516781299</v>
+        <v>5.4698908710432397</v>
       </c>
       <c r="G34" s="7">
-        <v>71.675702431157305</v>
+        <v>79.512131796377901</v>
       </c>
       <c r="H34" s="7">
-        <v>4.9272967448048499</v>
+        <v>4.9328570318447902</v>
       </c>
       <c r="I34" s="7">
-        <v>48.004748717890799</v>
+        <v>57.525703128952799</v>
       </c>
       <c r="J34" s="12">
         <f>SUM(C34:I34)</f>
-        <v>267.99999999999977</v>
+        <v>302</v>
       </c>
       <c r="K34" s="9">
         <f>C34/J34</f>
-        <v>0.3051158336587883</v>
+        <v>0.30838196979882881</v>
       </c>
       <c r="M34" s="3">
         <f>AVERAGE(K34:K40)</f>
-        <v>0.25897978162918428</v>
+        <v>0.26191313715552783</v>
       </c>
       <c r="N34" s="2" t="s">
         <v>12</v>
@@ -11312,37 +11312,37 @@
         <v>5</v>
       </c>
       <c r="C35" s="7">
-        <v>7.8707822001121297</v>
+        <v>7.0488887388642203</v>
       </c>
       <c r="D35" s="6">
-        <v>5.5943056897486096</v>
+        <v>5.8587881979173799</v>
       </c>
       <c r="E35" s="7">
-        <v>26.885573369103799</v>
+        <v>28.210289106604701</v>
       </c>
       <c r="F35" s="7">
-        <v>8.3990854992692405</v>
+        <v>8.5361285430581599</v>
       </c>
       <c r="G35" s="7">
-        <v>54.978506605184002</v>
+        <v>61.775334599553403</v>
       </c>
       <c r="H35" s="7">
-        <v>2.2327751143075698</v>
+        <v>2.5947115319475098</v>
       </c>
       <c r="I35" s="7">
-        <v>24.038971522274501</v>
+        <v>23.975859282054401</v>
       </c>
       <c r="J35" s="12">
         <f t="shared" ref="J35:J40" si="6">SUM(C35:I35)</f>
-        <v>129.99999999999986</v>
+        <v>137.99999999999977</v>
       </c>
       <c r="K35" s="9">
         <f>D35/J35</f>
-        <v>4.3033120690373967E-2</v>
+        <v>4.2454986941430357E-2</v>
       </c>
       <c r="M35" s="3">
         <f>AVERAGE(C42:I42)</f>
-        <v>0.25787659498955684</v>
+        <v>0.26739596051920628</v>
       </c>
       <c r="N35" s="2" t="s">
         <v>14</v>
@@ -11353,37 +11353,37 @@
         <v>6</v>
       </c>
       <c r="C36" s="7">
-        <v>52.787610528018497</v>
+        <v>52.354857727082901</v>
       </c>
       <c r="D36" s="7">
-        <v>30.026274113141699</v>
+        <v>28.2466689869206</v>
       </c>
       <c r="E36" s="6">
-        <v>193.44152264071599</v>
+        <v>186.720192866937</v>
       </c>
       <c r="F36" s="7">
-        <v>62.178481007739101</v>
+        <v>57.593815924399401</v>
       </c>
       <c r="G36" s="7">
-        <v>308.63420887321098</v>
+        <v>308.67590777268299</v>
       </c>
       <c r="H36" s="7">
-        <v>19.014383738054001</v>
+        <v>18.236870933511099</v>
       </c>
       <c r="I36" s="7">
-        <v>176.917519099119</v>
+        <v>171.171685788464</v>
       </c>
       <c r="J36" s="12">
         <f t="shared" si="6"/>
-        <v>842.9999999999992</v>
+        <v>822.99999999999795</v>
       </c>
       <c r="K36" s="9">
         <f>E36/J36</f>
-        <v>0.22946799838756365</v>
+        <v>0.22687751259652184</v>
       </c>
       <c r="M36" s="4">
         <f>2*M34*M35/(M34+M35)</f>
-        <v>0.25842701097963555</v>
+        <v>0.26462615205355078</v>
       </c>
       <c r="N36" s="2" t="s">
         <v>15</v>
@@ -11394,37 +11394,37 @@
         <v>7</v>
       </c>
       <c r="C37" s="7">
-        <v>5.4609981361901596</v>
+        <v>5.0392163822660896</v>
       </c>
       <c r="D37" s="7">
-        <v>9.7317565212867994</v>
+        <v>9.5204902371445197</v>
       </c>
       <c r="E37" s="7">
-        <v>63.996884778389202</v>
+        <v>65.708390978152096</v>
       </c>
       <c r="F37" s="6">
-        <v>89.331789948846705</v>
+        <v>92.024805344767501</v>
       </c>
       <c r="G37" s="7">
-        <v>93.856979092332907</v>
+        <v>97.125363028150005</v>
       </c>
       <c r="H37" s="7">
-        <v>8.0883595617594697</v>
+        <v>8.0433555139402397</v>
       </c>
       <c r="I37" s="7">
-        <v>60.533231961194502</v>
+        <v>61.538378515579502</v>
       </c>
       <c r="J37" s="12">
         <f t="shared" si="6"/>
-        <v>330.99999999999977</v>
+        <v>338.99999999999994</v>
       </c>
       <c r="K37" s="9">
         <f>F37/J37</f>
-        <v>0.26988456177899323</v>
+        <v>0.27145960278692483</v>
       </c>
       <c r="M37" s="4">
         <f>SUM(C34,D35,E36,F37,G38,H39,I40)/J41</f>
-        <v>0.37630594820937252</v>
+        <v>0.37719845395622725</v>
       </c>
       <c r="N37" s="2" t="s">
         <v>13</v>
@@ -11435,36 +11435,36 @@
         <v>8</v>
       </c>
       <c r="C38" s="7">
-        <v>72.047305318872802</v>
+        <v>61.273889196278503</v>
       </c>
       <c r="D38" s="7">
-        <v>60.356793594719697</v>
+        <v>60.157590708398601</v>
       </c>
       <c r="E38" s="7">
-        <v>282.83773343638597</v>
+        <v>277.60570950263099</v>
       </c>
       <c r="F38" s="7">
-        <v>85.948336441700803</v>
+        <v>83.061882692203994</v>
       </c>
       <c r="G38" s="6">
-        <v>930.27429812908997</v>
+        <v>924.84071100608901</v>
       </c>
       <c r="H38" s="7">
-        <v>29.218521443051198</v>
+        <v>29.206103194944699</v>
       </c>
       <c r="I38" s="7">
-        <v>261.31701163617498</v>
+        <v>259.85411369945501</v>
       </c>
       <c r="J38" s="12">
         <f t="shared" si="6"/>
-        <v>1721.9999999999955</v>
+        <v>1696.0000000000009</v>
       </c>
       <c r="K38" s="9">
         <f>G38/J38</f>
-        <v>0.54022897684616289</v>
+        <v>0.5453070229988729</v>
       </c>
       <c r="M38" s="4">
-        <v>0.37630594820937302</v>
+        <v>0.37719845395622598</v>
       </c>
       <c r="N38" s="2" t="s">
         <v>16</v>
@@ -11475,33 +11475,33 @@
         <v>9</v>
       </c>
       <c r="C39" s="7">
-        <v>4.8002810732440597</v>
+        <v>5.0146726620792101</v>
       </c>
       <c r="D39" s="7">
-        <v>2.4155745319811999</v>
+        <v>2.76175748082568</v>
       </c>
       <c r="E39" s="7">
-        <v>17.557279629278899</v>
+        <v>19.018040848718002</v>
       </c>
       <c r="F39" s="7">
-        <v>7.7667464928760603</v>
+        <v>8.0748503361678505</v>
       </c>
       <c r="G39" s="7">
-        <v>30.056025068777402</v>
+        <v>32.807459847831502</v>
       </c>
       <c r="H39" s="6">
-        <v>7.8692034274138498</v>
+        <v>9.3016054077474699</v>
       </c>
       <c r="I39" s="7">
-        <v>23.5348897764284</v>
+        <v>22.021613416630199</v>
       </c>
       <c r="J39" s="12">
         <f t="shared" si="6"/>
-        <v>93.999999999999872</v>
+        <v>98.999999999999915</v>
       </c>
       <c r="K39" s="9">
         <f>H39/J39</f>
-        <v>8.3714930078870861E-2</v>
+        <v>9.3955610179267457E-2</v>
       </c>
     </row>
     <row r="40" spans="2:14" x14ac:dyDescent="0.35">
@@ -11509,33 +11509,33 @@
         <v>10</v>
       </c>
       <c r="C40" s="7">
-        <v>64.553705217687906</v>
+        <v>52.8853833936383</v>
       </c>
       <c r="D40" s="7">
-        <v>24.158089934033299</v>
+        <v>24.9835307979242</v>
       </c>
       <c r="E40" s="7">
-        <v>176.336798669844</v>
+        <v>171.407532270893</v>
       </c>
       <c r="F40" s="7">
-        <v>60.570114980937198</v>
+        <v>58.743589079333503</v>
       </c>
       <c r="G40" s="7">
-        <v>281.09757694460399</v>
+        <v>289.04445053618201</v>
       </c>
       <c r="H40" s="7">
-        <v>22.892838487750399</v>
+        <v>23.262887638882301</v>
       </c>
       <c r="I40" s="6">
-        <v>326.390875765141</v>
+        <v>326.67262628314501</v>
       </c>
       <c r="J40" s="12">
         <f t="shared" si="6"/>
-        <v>955.99999999999784</v>
+        <v>946.99999999999818</v>
       </c>
       <c r="K40" s="9">
         <f>I40/J40</f>
-        <v>0.34141304996353738</v>
+        <v>0.34495525478684863</v>
       </c>
     </row>
     <row r="41" spans="2:14" x14ac:dyDescent="0.35">
@@ -11544,35 +11544,35 @@
       </c>
       <c r="C41" s="8">
         <f>SUM(C34:C40)</f>
-        <v>289.29172589468078</v>
+        <v>276.74826297945555</v>
       </c>
       <c r="D41" s="8">
         <f t="shared" ref="D41:I41" si="7">SUM(D34:D40)</f>
-        <v>138.65616425484831</v>
+        <v>138.17987703770478</v>
       </c>
       <c r="E41" s="8">
         <f t="shared" si="7"/>
-        <v>812.04692708769437</v>
+        <v>803.44716723789702</v>
       </c>
       <c r="F41" s="8">
         <f t="shared" si="7"/>
-        <v>318.45125862304724</v>
+        <v>313.50496279097365</v>
       </c>
       <c r="G41" s="8">
         <f t="shared" si="7"/>
-        <v>1770.5732971443567</v>
+        <v>1793.7813585868669</v>
       </c>
       <c r="H41" s="8">
         <f t="shared" si="7"/>
-        <v>94.243378517141338</v>
+        <v>95.578391252818122</v>
       </c>
       <c r="I41" s="8">
         <f t="shared" si="7"/>
-        <v>920.73724847822325</v>
+        <v>922.75998011428101</v>
       </c>
       <c r="J41" s="12">
         <f>SUM(J34:J40)</f>
-        <v>4343.9999999999918</v>
+        <v>4343.9999999999964</v>
       </c>
       <c r="K41" s="10"/>
     </row>
@@ -11582,31 +11582,31 @@
       </c>
       <c r="C42" s="9">
         <f>C34/C41</f>
-        <v>0.28265946137126879</v>
+        <v>0.33652010631105539</v>
       </c>
       <c r="D42" s="9">
         <f>IFERROR(D35/D41, 0)</f>
-        <v>4.0346606440564342E-2</v>
+        <v>4.2399720737330712E-2</v>
       </c>
       <c r="E42" s="9">
         <f>IFERROR(E36/E41, 0)</f>
-        <v>0.23821470925882329</v>
+        <v>0.2323988439822951</v>
       </c>
       <c r="F42" s="9">
         <f>IFERROR(F37/F41, 0)</f>
-        <v>0.28051950661180869</v>
+        <v>0.29353540220071134</v>
       </c>
       <c r="G42" s="9">
         <f>IFERROR(G38/G41, 0)</f>
-        <v>0.52540852142606542</v>
+        <v>0.51558162681246422</v>
       </c>
       <c r="H42" s="9">
         <f>IFERROR(H39/H41, 0)</f>
-        <v>8.3498740720363396E-2</v>
+        <v>9.7319125022134259E-2</v>
       </c>
       <c r="I42" s="9">
         <f>IFERROR(I40/I41, 0)</f>
-        <v>0.35448861909800383</v>
+        <v>0.35401689856845286</v>
       </c>
       <c r="J42" s="10"/>
       <c r="K42" s="10"/>
@@ -11617,31 +11617,31 @@
       </c>
       <c r="C43" s="7">
         <f>C41-J34</f>
-        <v>21.291725894681008</v>
+        <v>-25.251737020544454</v>
       </c>
       <c r="D43" s="7">
         <f>D41-J35</f>
-        <v>8.6561642548484485</v>
+        <v>0.17987703770501184</v>
       </c>
       <c r="E43" s="7">
         <f>E41-J36</f>
-        <v>-30.953072912304833</v>
+        <v>-19.552832762100934</v>
       </c>
       <c r="F43" s="7">
         <f>F41-J37</f>
-        <v>-12.548741376952535</v>
+        <v>-25.495037209026293</v>
       </c>
       <c r="G43" s="7">
         <f>G41-J38</f>
-        <v>48.573297144361277</v>
+        <v>97.781358586865963</v>
       </c>
       <c r="H43" s="7">
         <f>H41-J39</f>
-        <v>0.24337851714146552</v>
+        <v>-3.4216087471817929</v>
       </c>
       <c r="I43" s="7">
         <f>I41-J40</f>
-        <v>-35.262751521774589</v>
+        <v>-24.240019885717174</v>
       </c>
       <c r="J43" s="10"/>
       <c r="K43" s="10"/>
@@ -11652,31 +11652,31 @@
       </c>
       <c r="C44" s="9">
         <f>C43/$J41</f>
-        <v>4.9014101967497807E-3</v>
+        <v>-5.8130149678969787E-3</v>
       </c>
       <c r="D44" s="9">
         <f t="shared" ref="D44:I44" si="8">D43/$J41</f>
-        <v>1.9926713293850059E-3</v>
+        <v>4.140815785106169E-5</v>
       </c>
       <c r="E44" s="9">
         <f t="shared" si="8"/>
-        <v>-7.1254771897571109E-3</v>
+        <v>-4.5011125142957985E-3</v>
       </c>
       <c r="F44" s="9">
         <f t="shared" si="8"/>
-        <v>-2.8887526190038118E-3</v>
+        <v>-5.8690232985788016E-3</v>
       </c>
       <c r="G44" s="9">
         <f t="shared" si="8"/>
-        <v>1.1181698237652249E-2</v>
+        <v>2.250952085333012E-2</v>
       </c>
       <c r="H44" s="9">
         <f t="shared" si="8"/>
-        <v>5.6026362141221452E-5</v>
+        <v>-7.8766315542859022E-4</v>
       </c>
       <c r="I44" s="9">
         <f t="shared" si="8"/>
-        <v>-8.1175763171672782E-3</v>
+        <v>-5.5801150749809382E-3</v>
       </c>
       <c r="J44" s="10"/>
       <c r="K44" s="10"/>

</xml_diff>